<commit_message>
PMO-2235: applying ceded share
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/PMO-2235_Spec.xlsx
+++ b/test/data/spreadsheets/PMO-2235_Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="22944" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="22944" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="StopLoss" sheetId="1" r:id="rId1"/>
@@ -602,46 +602,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <b val="0"/>
@@ -2588,9 +2549,9 @@
   </sheetPr>
   <dimension ref="A2:AK100"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -2620,7 +2581,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="2">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -8236,22 +8197,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D31:D40 D18:D27 D46:D55">
-    <cfRule type="expression" dxfId="20" priority="51">
+    <cfRule type="expression" dxfId="17" priority="51">
       <formula>$U18=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:R27">
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>$U18=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:R55">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>$U46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:R40">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>$U31=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8271,9 +8232,9 @@
   </sheetPr>
   <dimension ref="A2:AK183"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K163" sqref="K163:M163"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -8303,7 +8264,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="2">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -16053,7 +16014,7 @@
         <v>0</v>
       </c>
       <c r="F156" s="42">
-        <f t="shared" ref="E156:G156" si="122">SUM(F103:F107)+E156</f>
+        <f t="shared" ref="F156:G156" si="122">SUM(F103:F107)+E156</f>
         <v>0</v>
       </c>
       <c r="G156" s="42">
@@ -16883,72 +16844,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D31:D40 D18:D27 D56:D65">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$U18=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:R27">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$U18=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:R65">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$U56=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:R40">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$U31=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:D53">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$U44=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:R53">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$U44=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89:D112">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$U89=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E89:R112">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$U89=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D116:D125">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$U116=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E116:R125">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$U116=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D143:D168">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$U143=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E143:R168">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$U143=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D174:D183">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$U174=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E174:R183">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$U174=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
PMO-2235: introduced premium calculation for retro contract
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/PMO-2235_Spec.xlsx
+++ b/test/data/spreadsheets/PMO-2235_Spec.xlsx
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="69">
   <si>
     <t>DY</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>reported reserves, ceded (incremental)</t>
+  </si>
+  <si>
+    <t>Premium</t>
   </si>
 </sst>
 </file>
@@ -2550,8 +2553,8 @@
   <dimension ref="A2:AK100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -2633,7 +2636,12 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="D10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10">
+        <v>200</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="D11" s="18" t="s">

</xml_diff>